<commit_message>
Accessing the generator and tasl
</commit_message>
<xml_diff>
--- a/table_data.xlsx
+++ b/table_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N121"/>
+  <dimension ref="A1:N161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5785,6 +5785,1766 @@
         <v>-125.3184402119656</v>
       </c>
     </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>1</v>
+      </c>
+      <c r="B122" t="n">
+        <v>3.447025272688801</v>
+      </c>
+      <c r="C122" t="n">
+        <v>9.701259730204788</v>
+      </c>
+      <c r="D122" t="n">
+        <v>-1.931881545166662</v>
+      </c>
+      <c r="E122" t="n">
+        <v>25.53534878581116</v>
+      </c>
+      <c r="F122" t="n">
+        <v>17.73647181191756</v>
+      </c>
+      <c r="G122" t="n">
+        <v>-32.47072003175676</v>
+      </c>
+      <c r="H122" t="n">
+        <v>-72.05238358535804</v>
+      </c>
+      <c r="I122" t="n">
+        <v>6.330021481421864</v>
+      </c>
+      <c r="J122" t="n">
+        <v>25.59254609436162</v>
+      </c>
+      <c r="K122" t="n">
+        <v>-51.67604733614606</v>
+      </c>
+      <c r="L122" t="n">
+        <v>-64.19630930291399</v>
+      </c>
+      <c r="M122" t="n">
+        <v>-16.57026598178296</v>
+      </c>
+      <c r="N122" t="n">
+        <v>-125.3184402119656</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>2</v>
+      </c>
+      <c r="B123" t="n">
+        <v>3.777719236224569</v>
+      </c>
+      <c r="C123" t="n">
+        <v>11.1570715082183</v>
+      </c>
+      <c r="D123" t="n">
+        <v>-4.792320145917249</v>
+      </c>
+      <c r="E123" t="n">
+        <v>24.93477471535802</v>
+      </c>
+      <c r="F123" t="n">
+        <v>16.36748595754155</v>
+      </c>
+      <c r="G123" t="n">
+        <v>-25.53799940980731</v>
+      </c>
+      <c r="H123" t="n">
+        <v>-77.51612136910649</v>
+      </c>
+      <c r="I123" t="n">
+        <v>6.148335208007468</v>
+      </c>
+      <c r="J123" t="n">
+        <v>25.17839911320585</v>
+      </c>
+      <c r="K123" t="n">
+        <v>-44.32443891715786</v>
+      </c>
+      <c r="L123" t="n">
+        <v>-68.70520821344219</v>
+      </c>
+      <c r="M123" t="n">
+        <v>-12.33337838262858</v>
+      </c>
+      <c r="N123" t="n">
+        <v>-131.5136695641207</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>3</v>
+      </c>
+      <c r="B124" t="n">
+        <v>4.108413199760336</v>
+      </c>
+      <c r="C124" t="n">
+        <v>13.46278628389064</v>
+      </c>
+      <c r="D124" t="n">
+        <v>-7.025070981750273</v>
+      </c>
+      <c r="E124" t="n">
+        <v>24.58350756153641</v>
+      </c>
+      <c r="F124" t="n">
+        <v>15.64411643784896</v>
+      </c>
+      <c r="G124" t="n">
+        <v>-16.15576840607682</v>
+      </c>
+      <c r="H124" t="n">
+        <v>-83.04553807179916</v>
+      </c>
+      <c r="I124" t="n">
+        <v>6.042069514414376</v>
+      </c>
+      <c r="J124" t="n">
+        <v>24.95956463666019</v>
+      </c>
+      <c r="K124" t="n">
+        <v>-34.69720645319886</v>
+      </c>
+      <c r="L124" t="n">
+        <v>-73.73008987298792</v>
+      </c>
+      <c r="M124" t="n">
+        <v>-4.415399442497812</v>
+      </c>
+      <c r="N124" t="n">
+        <v>-137.3802504032666</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>4</v>
+      </c>
+      <c r="B125" t="n">
+        <v>4.439107163296104</v>
+      </c>
+      <c r="C125" t="n">
+        <v>16.36854408442674</v>
+      </c>
+      <c r="D125" t="n">
+        <v>-8.388180854904453</v>
+      </c>
+      <c r="E125" t="n">
+        <v>24.51627503200149</v>
+      </c>
+      <c r="F125" t="n">
+        <v>15.51112834862551</v>
+      </c>
+      <c r="G125" t="n">
+        <v>-5.331848241292139</v>
+      </c>
+      <c r="H125" t="n">
+        <v>-87.55192480501077</v>
+      </c>
+      <c r="I125" t="n">
+        <v>6.021730261781963</v>
+      </c>
+      <c r="J125" t="n">
+        <v>24.91933294580268</v>
+      </c>
+      <c r="K125" t="n">
+        <v>-23.82639301151166</v>
+      </c>
+      <c r="L125" t="n">
+        <v>-78.14372020783361</v>
+      </c>
+      <c r="M125" t="n">
+        <v>6.136213220836726</v>
+      </c>
+      <c r="N125" t="n">
+        <v>-141.9447625122414</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>5</v>
+      </c>
+      <c r="B126" t="n">
+        <v>4.769801126831871</v>
+      </c>
+      <c r="C126" t="n">
+        <v>19.55946096466073</v>
+      </c>
+      <c r="D126" t="n">
+        <v>-8.733935659794598</v>
+      </c>
+      <c r="E126" t="n">
+        <v>24.74824388666533</v>
+      </c>
+      <c r="F126" t="n">
+        <v>15.97717584471514</v>
+      </c>
+      <c r="G126" t="n">
+        <v>5.739831202094024</v>
+      </c>
+      <c r="H126" t="n">
+        <v>-90.52585402642181</v>
+      </c>
+      <c r="I126" t="n">
+        <v>6.091905713613039</v>
+      </c>
+      <c r="J126" t="n">
+        <v>25.06032210428357</v>
+      </c>
+      <c r="K126" t="n">
+        <v>-12.91650697095826</v>
+      </c>
+      <c r="L126" t="n">
+        <v>-81.44270776685337</v>
+      </c>
+      <c r="M126" t="n">
+        <v>18.15790386470075</v>
+      </c>
+      <c r="N126" t="n">
+        <v>-144.7096957035354</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>6</v>
+      </c>
+      <c r="B127" t="n">
+        <v>5.100495090367639</v>
+      </c>
+      <c r="C127" t="n">
+        <v>22.68975156844244</v>
+      </c>
+      <c r="D127" t="n">
+        <v>-8.024867498372293</v>
+      </c>
+      <c r="E127" t="n">
+        <v>25.26353752912881</v>
+      </c>
+      <c r="F127" t="n">
+        <v>17.09361425965945</v>
+      </c>
+      <c r="G127" t="n">
+        <v>15.83481668305001</v>
+      </c>
+      <c r="H127" t="n">
+        <v>-92.01820049972025</v>
+      </c>
+      <c r="I127" t="n">
+        <v>6.247792865954933</v>
+      </c>
+      <c r="J127" t="n">
+        <v>25.39806817939277</v>
+      </c>
+      <c r="K127" t="n">
+        <v>-3.180927980123869</v>
+      </c>
+      <c r="L127" t="n">
+        <v>-83.71374657998693</v>
+      </c>
+      <c r="M127" t="n">
+        <v>30.4813156246775</v>
+      </c>
+      <c r="N127" t="n">
+        <v>-145.6426100190539</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>7</v>
+      </c>
+      <c r="B128" t="n">
+        <v>5.431189053903407</v>
+      </c>
+      <c r="C128" t="n">
+        <v>25.4202003373889</v>
+      </c>
+      <c r="D128" t="n">
+        <v>-6.337814908253783</v>
+      </c>
+      <c r="E128" t="n">
+        <v>25.98519077674523</v>
+      </c>
+      <c r="F128" t="n">
+        <v>18.90586322714154</v>
+      </c>
+      <c r="G128" t="n">
+        <v>23.91542382068737</v>
+      </c>
+      <c r="H128" t="n">
+        <v>-92.47684069402248</v>
+      </c>
+      <c r="I128" t="n">
+        <v>6.466108134141415</v>
+      </c>
+      <c r="J128" t="n">
+        <v>25.94631156451341</v>
+      </c>
+      <c r="K128" t="n">
+        <v>4.396341178083549</v>
+      </c>
+      <c r="L128" t="n">
+        <v>-85.43639235665063</v>
+      </c>
+      <c r="M128" t="n">
+        <v>42.04459514683843</v>
+      </c>
+      <c r="N128" t="n">
+        <v>-145.0261544342737</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>8</v>
+      </c>
+      <c r="B129" t="n">
+        <v>5.761883017439175</v>
+      </c>
+      <c r="C129" t="n">
+        <v>27.45492078010687</v>
+      </c>
+      <c r="D129" t="n">
+        <v>-3.855596214896483</v>
+      </c>
+      <c r="E129" t="n">
+        <v>26.7588481016521</v>
+      </c>
+      <c r="F129" t="n">
+        <v>21.38480756210971</v>
+      </c>
+      <c r="G129" t="n">
+        <v>29.30881731975372</v>
+      </c>
+      <c r="H129" t="n">
+        <v>-92.46484551972567</v>
+      </c>
+      <c r="I129" t="n">
+        <v>6.700155728230888</v>
+      </c>
+      <c r="J129" t="n">
+        <v>26.69624430450378</v>
+      </c>
+      <c r="K129" t="n">
+        <v>9.250124946332502</v>
+      </c>
+      <c r="L129" t="n">
+        <v>-87.15340877733161</v>
+      </c>
+      <c r="M129" t="n">
+        <v>51.95155884910947</v>
+      </c>
+      <c r="N129" t="n">
+        <v>-143.2329800489664</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>9</v>
+      </c>
+      <c r="B130" t="n">
+        <v>6.092576980974942</v>
+      </c>
+      <c r="C130" t="n">
+        <v>28.57341936468722</v>
+      </c>
+      <c r="D130" t="n">
+        <v>-0.8471983293170848</v>
+      </c>
+      <c r="E130" t="n">
+        <v>27.38829075065058</v>
+      </c>
+      <c r="F130" t="n">
+        <v>24.37497386437376</v>
+      </c>
+      <c r="G130" t="n">
+        <v>31.72985101989372</v>
+      </c>
+      <c r="H130" t="n">
+        <v>-92.39805655114469</v>
+      </c>
+      <c r="I130" t="n">
+        <v>6.890575353137988</v>
+      </c>
+      <c r="J130" t="n">
+        <v>27.60083242955845</v>
+      </c>
+      <c r="K130" t="n">
+        <v>11.23213562238114</v>
+      </c>
+      <c r="L130" t="n">
+        <v>-89.17219798596</v>
+      </c>
+      <c r="M130" t="n">
+        <v>59.46079705231288</v>
+      </c>
+      <c r="N130" t="n">
+        <v>-140.5757677845704</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>10</v>
+      </c>
+      <c r="B131" t="n">
+        <v>6.42327094451071</v>
+      </c>
+      <c r="C131" t="n">
+        <v>28.65448941419694</v>
+      </c>
+      <c r="D131" t="n">
+        <v>2.361372157479072</v>
+      </c>
+      <c r="E131" t="n">
+        <v>27.71675508625803</v>
+      </c>
+      <c r="F131" t="n">
+        <v>27.59395336373311</v>
+      </c>
+      <c r="G131" t="n">
+        <v>31.15201945593522</v>
+      </c>
+      <c r="H131" t="n">
+        <v>-92.43618857736628</v>
+      </c>
+      <c r="I131" t="n">
+        <v>6.989942715170496</v>
+      </c>
+      <c r="J131" t="n">
+        <v>28.57464135373439</v>
+      </c>
+      <c r="K131" t="n">
+        <v>10.42520708484769</v>
+      </c>
+      <c r="L131" t="n">
+        <v>-91.45550058736501</v>
+      </c>
+      <c r="M131" t="n">
+        <v>63.95113646381277</v>
+      </c>
+      <c r="N131" t="n">
+        <v>-137.3173110126157</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>11</v>
+      </c>
+      <c r="B132" t="n">
+        <v>6.753964908046478</v>
+      </c>
+      <c r="C132" t="n">
+        <v>27.68934573084024</v>
+      </c>
+      <c r="D132" t="n">
+        <v>5.42241684714688</v>
+      </c>
+      <c r="E132" t="n">
+        <v>27.70295497348244</v>
+      </c>
+      <c r="F132" t="n">
+        <v>30.67241317959246</v>
+      </c>
+      <c r="G132" t="n">
+        <v>27.6530993321199</v>
+      </c>
+      <c r="H132" t="n">
+        <v>-92.49998656440459</v>
+      </c>
+      <c r="I132" t="n">
+        <v>6.985767891137545</v>
+      </c>
+      <c r="J132" t="n">
+        <v>29.50594012155738</v>
+      </c>
+      <c r="K132" t="n">
+        <v>6.935912249775004</v>
+      </c>
+      <c r="L132" t="n">
+        <v>-93.66645962243966</v>
+      </c>
+      <c r="M132" t="n">
+        <v>64.91463148210208</v>
+      </c>
+      <c r="N132" t="n">
+        <v>-133.7513556250811</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>12</v>
+      </c>
+      <c r="B133" t="n">
+        <v>7.084658871582246</v>
+      </c>
+      <c r="C133" t="n">
+        <v>25.78257660845605</v>
+      </c>
+      <c r="D133" t="n">
+        <v>8.004224050558687</v>
+      </c>
+      <c r="E133" t="n">
+        <v>27.45218503889162</v>
+      </c>
+      <c r="F133" t="n">
+        <v>33.19896373345715</v>
+      </c>
+      <c r="G133" t="n">
+        <v>21.33579771947419</v>
+      </c>
+      <c r="H133" t="n">
+        <v>-92.29756121457852</v>
+      </c>
+      <c r="I133" t="n">
+        <v>6.909904717647885</v>
+      </c>
+      <c r="J133" t="n">
+        <v>30.2702747428946</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.7935173982304526</v>
+      </c>
+      <c r="L133" t="n">
+        <v>-95.22625020514107</v>
+      </c>
+      <c r="M133" t="n">
+        <v>61.97895669814836</v>
+      </c>
+      <c r="N133" t="n">
+        <v>-130.22157545066</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>13</v>
+      </c>
+      <c r="B134" t="n">
+        <v>7.415352835118012</v>
+      </c>
+      <c r="C134" t="n">
+        <v>23.14081006802608</v>
+      </c>
+      <c r="D134" t="n">
+        <v>9.827014896358444</v>
+      </c>
+      <c r="E134" t="n">
+        <v>27.18896083043538</v>
+      </c>
+      <c r="F134" t="n">
+        <v>34.75039699840882</v>
+      </c>
+      <c r="G134" t="n">
+        <v>12.35910160180724</v>
+      </c>
+      <c r="H134" t="n">
+        <v>-91.3034789877093</v>
+      </c>
+      <c r="I134" t="n">
+        <v>6.830273864669527</v>
+      </c>
+      <c r="J134" t="n">
+        <v>30.7396158986783</v>
+      </c>
+      <c r="K134" t="n">
+        <v>-7.999585363958612</v>
+      </c>
+      <c r="L134" t="n">
+        <v>-95.31426008743982</v>
+      </c>
+      <c r="M134" t="n">
+        <v>54.95066653435794</v>
+      </c>
+      <c r="N134" t="n">
+        <v>-127.0254025661032</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>14</v>
+      </c>
+      <c r="B135" t="n">
+        <v>7.746046798653781</v>
+      </c>
+      <c r="C135" t="n">
+        <v>20.05032250543721</v>
+      </c>
+      <c r="D135" t="n">
+        <v>10.69326171288964</v>
+      </c>
+      <c r="E135" t="n">
+        <v>27.15436389024016</v>
+      </c>
+      <c r="F135" t="n">
+        <v>34.92330702863362</v>
+      </c>
+      <c r="G135" t="n">
+        <v>1.129657827100637</v>
+      </c>
+      <c r="H135" t="n">
+        <v>-88.7635323448047</v>
+      </c>
+      <c r="I135" t="n">
+        <v>6.819807563433999</v>
+      </c>
+      <c r="J135" t="n">
+        <v>30.79192481538496</v>
+      </c>
+      <c r="K135" t="n">
+        <v>-19.20489849970553</v>
+      </c>
+      <c r="L135" t="n">
+        <v>-92.89491455805336</v>
+      </c>
+      <c r="M135" t="n">
+        <v>43.93220829822495</v>
+      </c>
+      <c r="N135" t="n">
+        <v>-124.2323764295948</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>15</v>
+      </c>
+      <c r="B136" t="n">
+        <v>8.076740762189548</v>
+      </c>
+      <c r="C136" t="n">
+        <v>16.84601620195139</v>
+      </c>
+      <c r="D136" t="n">
+        <v>10.50909321637684</v>
+      </c>
+      <c r="E136" t="n">
+        <v>27.41683350686776</v>
+      </c>
+      <c r="F136" t="n">
+        <v>33.43986558684183</v>
+      </c>
+      <c r="G136" t="n">
+        <v>-11.30794275866747</v>
+      </c>
+      <c r="H136" t="n">
+        <v>-84.00381957497078</v>
+      </c>
+      <c r="I136" t="n">
+        <v>6.899210136531421</v>
+      </c>
+      <c r="J136" t="n">
+        <v>30.34315261450677</v>
+      </c>
+      <c r="K136" t="n">
+        <v>-31.8255661290038</v>
+      </c>
+      <c r="L136" t="n">
+        <v>-87.10053254730583</v>
+      </c>
+      <c r="M136" t="n">
+        <v>29.64423263539317</v>
+      </c>
+      <c r="N136" t="n">
+        <v>-121.5939320786384</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>16</v>
+      </c>
+      <c r="B137" t="n">
+        <v>8.407434725725317</v>
+      </c>
+      <c r="C137" t="n">
+        <v>13.87512746548638</v>
+      </c>
+      <c r="D137" t="n">
+        <v>9.294466921085883</v>
+      </c>
+      <c r="E137" t="n">
+        <v>27.71643859312513</v>
+      </c>
+      <c r="F137" t="n">
+        <v>30.41271983812198</v>
+      </c>
+      <c r="G137" t="n">
+        <v>-22.9893546467396</v>
+      </c>
+      <c r="H137" t="n">
+        <v>-77.36389682478573</v>
+      </c>
+      <c r="I137" t="n">
+        <v>6.989846969348777</v>
+      </c>
+      <c r="J137" t="n">
+        <v>29.42737743002009</v>
+      </c>
+      <c r="K137" t="n">
+        <v>-43.71594627051596</v>
+      </c>
+      <c r="L137" t="n">
+        <v>-78.34923923288761</v>
+      </c>
+      <c r="M137" t="n">
+        <v>13.91018148157017</v>
+      </c>
+      <c r="N137" t="n">
+        <v>-118.9393879350523</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>17</v>
+      </c>
+      <c r="B138" t="n">
+        <v>8.738128689261083</v>
+      </c>
+      <c r="C138" t="n">
+        <v>11.4595981887266</v>
+      </c>
+      <c r="D138" t="n">
+        <v>7.181006432980378</v>
+      </c>
+      <c r="E138" t="n">
+        <v>27.64956278225451</v>
+      </c>
+      <c r="F138" t="n">
+        <v>26.55747531821106</v>
+      </c>
+      <c r="G138" t="n">
+        <v>-31.66020850096656</v>
+      </c>
+      <c r="H138" t="n">
+        <v>-70.98310383698367</v>
+      </c>
+      <c r="I138" t="n">
+        <v>6.969615631606407</v>
+      </c>
+      <c r="J138" t="n">
+        <v>28.26108497021511</v>
+      </c>
+      <c r="K138" t="n">
+        <v>-52.34015565161467</v>
+      </c>
+      <c r="L138" t="n">
+        <v>-69.27949418497963</v>
+      </c>
+      <c r="M138" t="n">
+        <v>-0.4477646451716297</v>
+      </c>
+      <c r="N138" t="n">
+        <v>-116.9818057327236</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>18</v>
+      </c>
+      <c r="B139" t="n">
+        <v>9.068822652796852</v>
+      </c>
+      <c r="C139" t="n">
+        <v>9.861188449607457</v>
+      </c>
+      <c r="D139" t="n">
+        <v>4.397737989664864</v>
+      </c>
+      <c r="E139" t="n">
+        <v>27.10568952294837</v>
+      </c>
+      <c r="F139" t="n">
+        <v>22.84196968229831</v>
+      </c>
+      <c r="G139" t="n">
+        <v>-36.06723520117182</v>
+      </c>
+      <c r="H139" t="n">
+        <v>-67.56797748786511</v>
+      </c>
+      <c r="I139" t="n">
+        <v>6.805082544757491</v>
+      </c>
+      <c r="J139" t="n">
+        <v>27.13706645851041</v>
+      </c>
+      <c r="K139" t="n">
+        <v>-56.3678421793627</v>
+      </c>
+      <c r="L139" t="n">
+        <v>-63.272880711653</v>
+      </c>
+      <c r="M139" t="n">
+        <v>-10.8978968733922</v>
+      </c>
+      <c r="N139" t="n">
+        <v>-117.1320938997014</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>19</v>
+      </c>
+      <c r="B140" t="n">
+        <v>9.399516616332619</v>
+      </c>
+      <c r="C140" t="n">
+        <v>9.253110745245055</v>
+      </c>
+      <c r="D140" t="n">
+        <v>1.2462719138322</v>
+      </c>
+      <c r="E140" t="n">
+        <v>26.31194193651951</v>
+      </c>
+      <c r="F140" t="n">
+        <v>19.86236114835194</v>
+      </c>
+      <c r="G140" t="n">
+        <v>-36.18080599191165</v>
+      </c>
+      <c r="H140" t="n">
+        <v>-68.19755462150795</v>
+      </c>
+      <c r="I140" t="n">
+        <v>6.564957224493295</v>
+      </c>
+      <c r="J140" t="n">
+        <v>26.2356722801737</v>
+      </c>
+      <c r="K140" t="n">
+        <v>-55.92779070393787</v>
+      </c>
+      <c r="L140" t="n">
+        <v>-61.82424348968619</v>
+      </c>
+      <c r="M140" t="n">
+        <v>-16.27696982803617</v>
+      </c>
+      <c r="N140" t="n">
+        <v>-120.1006810543722</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>20</v>
+      </c>
+      <c r="B141" t="n">
+        <v>9.730210579868388</v>
+      </c>
+      <c r="C141" t="n">
+        <v>9.701259730204789</v>
+      </c>
+      <c r="D141" t="n">
+        <v>-1.931881545166664</v>
+      </c>
+      <c r="E141" t="n">
+        <v>25.53534878581116</v>
+      </c>
+      <c r="F141" t="n">
+        <v>17.73647181191756</v>
+      </c>
+      <c r="G141" t="n">
+        <v>-32.47072003175674</v>
+      </c>
+      <c r="H141" t="n">
+        <v>-72.05238358535806</v>
+      </c>
+      <c r="I141" t="n">
+        <v>6.330021481421864</v>
+      </c>
+      <c r="J141" t="n">
+        <v>25.59254609436162</v>
+      </c>
+      <c r="K141" t="n">
+        <v>-51.67604733614604</v>
+      </c>
+      <c r="L141" t="n">
+        <v>-64.196309302914</v>
+      </c>
+      <c r="M141" t="n">
+        <v>-16.57026598178295</v>
+      </c>
+      <c r="N141" t="n">
+        <v>-125.3184402119656</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>1</v>
+      </c>
+      <c r="B142" t="n">
+        <v>3.447025272688801</v>
+      </c>
+      <c r="C142" t="n">
+        <v>9.701259730204788</v>
+      </c>
+      <c r="D142" t="n">
+        <v>-1.931881545166662</v>
+      </c>
+      <c r="E142" t="n">
+        <v>25.53534878581116</v>
+      </c>
+      <c r="F142" t="n">
+        <v>17.73647181191756</v>
+      </c>
+      <c r="G142" t="n">
+        <v>-32.47072003175676</v>
+      </c>
+      <c r="H142" t="n">
+        <v>-72.05238358535804</v>
+      </c>
+      <c r="I142" t="n">
+        <v>6.330021481421864</v>
+      </c>
+      <c r="J142" t="n">
+        <v>25.59254609436162</v>
+      </c>
+      <c r="K142" t="n">
+        <v>-51.67604733614606</v>
+      </c>
+      <c r="L142" t="n">
+        <v>-64.19630930291399</v>
+      </c>
+      <c r="M142" t="n">
+        <v>-16.57026598178296</v>
+      </c>
+      <c r="N142" t="n">
+        <v>-125.3184402119656</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>2</v>
+      </c>
+      <c r="B143" t="n">
+        <v>3.777719236224569</v>
+      </c>
+      <c r="C143" t="n">
+        <v>11.1570715082183</v>
+      </c>
+      <c r="D143" t="n">
+        <v>-4.792320145917249</v>
+      </c>
+      <c r="E143" t="n">
+        <v>24.93477471535802</v>
+      </c>
+      <c r="F143" t="n">
+        <v>16.36748595754155</v>
+      </c>
+      <c r="G143" t="n">
+        <v>-25.53799940980731</v>
+      </c>
+      <c r="H143" t="n">
+        <v>-77.51612136910649</v>
+      </c>
+      <c r="I143" t="n">
+        <v>6.148335208007468</v>
+      </c>
+      <c r="J143" t="n">
+        <v>25.17839911320585</v>
+      </c>
+      <c r="K143" t="n">
+        <v>-44.32443891715786</v>
+      </c>
+      <c r="L143" t="n">
+        <v>-68.70520821344219</v>
+      </c>
+      <c r="M143" t="n">
+        <v>-12.33337838262858</v>
+      </c>
+      <c r="N143" t="n">
+        <v>-131.5136695641207</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>3</v>
+      </c>
+      <c r="B144" t="n">
+        <v>4.108413199760336</v>
+      </c>
+      <c r="C144" t="n">
+        <v>13.46278628389064</v>
+      </c>
+      <c r="D144" t="n">
+        <v>-7.025070981750273</v>
+      </c>
+      <c r="E144" t="n">
+        <v>24.58350756153641</v>
+      </c>
+      <c r="F144" t="n">
+        <v>15.64411643784896</v>
+      </c>
+      <c r="G144" t="n">
+        <v>-16.15576840607682</v>
+      </c>
+      <c r="H144" t="n">
+        <v>-83.04553807179916</v>
+      </c>
+      <c r="I144" t="n">
+        <v>6.042069514414376</v>
+      </c>
+      <c r="J144" t="n">
+        <v>24.95956463666019</v>
+      </c>
+      <c r="K144" t="n">
+        <v>-34.69720645319886</v>
+      </c>
+      <c r="L144" t="n">
+        <v>-73.73008987298792</v>
+      </c>
+      <c r="M144" t="n">
+        <v>-4.415399442497812</v>
+      </c>
+      <c r="N144" t="n">
+        <v>-137.3802504032666</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>4</v>
+      </c>
+      <c r="B145" t="n">
+        <v>4.439107163296104</v>
+      </c>
+      <c r="C145" t="n">
+        <v>16.36854408442674</v>
+      </c>
+      <c r="D145" t="n">
+        <v>-8.388180854904453</v>
+      </c>
+      <c r="E145" t="n">
+        <v>24.51627503200149</v>
+      </c>
+      <c r="F145" t="n">
+        <v>15.51112834862551</v>
+      </c>
+      <c r="G145" t="n">
+        <v>-5.331848241292139</v>
+      </c>
+      <c r="H145" t="n">
+        <v>-87.55192480501077</v>
+      </c>
+      <c r="I145" t="n">
+        <v>6.021730261781963</v>
+      </c>
+      <c r="J145" t="n">
+        <v>24.91933294580268</v>
+      </c>
+      <c r="K145" t="n">
+        <v>-23.82639301151166</v>
+      </c>
+      <c r="L145" t="n">
+        <v>-78.14372020783361</v>
+      </c>
+      <c r="M145" t="n">
+        <v>6.136213220836726</v>
+      </c>
+      <c r="N145" t="n">
+        <v>-141.9447625122414</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>5</v>
+      </c>
+      <c r="B146" t="n">
+        <v>4.769801126831871</v>
+      </c>
+      <c r="C146" t="n">
+        <v>19.55946096466073</v>
+      </c>
+      <c r="D146" t="n">
+        <v>-8.733935659794598</v>
+      </c>
+      <c r="E146" t="n">
+        <v>24.74824388666533</v>
+      </c>
+      <c r="F146" t="n">
+        <v>15.97717584471514</v>
+      </c>
+      <c r="G146" t="n">
+        <v>5.739831202094024</v>
+      </c>
+      <c r="H146" t="n">
+        <v>-90.52585402642181</v>
+      </c>
+      <c r="I146" t="n">
+        <v>6.091905713613039</v>
+      </c>
+      <c r="J146" t="n">
+        <v>25.06032210428357</v>
+      </c>
+      <c r="K146" t="n">
+        <v>-12.91650697095826</v>
+      </c>
+      <c r="L146" t="n">
+        <v>-81.44270776685337</v>
+      </c>
+      <c r="M146" t="n">
+        <v>18.15790386470075</v>
+      </c>
+      <c r="N146" t="n">
+        <v>-144.7096957035354</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>6</v>
+      </c>
+      <c r="B147" t="n">
+        <v>5.100495090367639</v>
+      </c>
+      <c r="C147" t="n">
+        <v>22.68975156844244</v>
+      </c>
+      <c r="D147" t="n">
+        <v>-8.024867498372293</v>
+      </c>
+      <c r="E147" t="n">
+        <v>25.26353752912881</v>
+      </c>
+      <c r="F147" t="n">
+        <v>17.09361425965945</v>
+      </c>
+      <c r="G147" t="n">
+        <v>15.83481668305001</v>
+      </c>
+      <c r="H147" t="n">
+        <v>-92.01820049972025</v>
+      </c>
+      <c r="I147" t="n">
+        <v>6.247792865954933</v>
+      </c>
+      <c r="J147" t="n">
+        <v>25.39806817939277</v>
+      </c>
+      <c r="K147" t="n">
+        <v>-3.180927980123869</v>
+      </c>
+      <c r="L147" t="n">
+        <v>-83.71374657998693</v>
+      </c>
+      <c r="M147" t="n">
+        <v>30.4813156246775</v>
+      </c>
+      <c r="N147" t="n">
+        <v>-145.6426100190539</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>7</v>
+      </c>
+      <c r="B148" t="n">
+        <v>5.431189053903407</v>
+      </c>
+      <c r="C148" t="n">
+        <v>25.4202003373889</v>
+      </c>
+      <c r="D148" t="n">
+        <v>-6.337814908253783</v>
+      </c>
+      <c r="E148" t="n">
+        <v>25.98519077674523</v>
+      </c>
+      <c r="F148" t="n">
+        <v>18.90586322714154</v>
+      </c>
+      <c r="G148" t="n">
+        <v>23.91542382068737</v>
+      </c>
+      <c r="H148" t="n">
+        <v>-92.47684069402248</v>
+      </c>
+      <c r="I148" t="n">
+        <v>6.466108134141415</v>
+      </c>
+      <c r="J148" t="n">
+        <v>25.94631156451341</v>
+      </c>
+      <c r="K148" t="n">
+        <v>4.396341178083549</v>
+      </c>
+      <c r="L148" t="n">
+        <v>-85.43639235665063</v>
+      </c>
+      <c r="M148" t="n">
+        <v>42.04459514683843</v>
+      </c>
+      <c r="N148" t="n">
+        <v>-145.0261544342737</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>8</v>
+      </c>
+      <c r="B149" t="n">
+        <v>5.761883017439175</v>
+      </c>
+      <c r="C149" t="n">
+        <v>27.45492078010687</v>
+      </c>
+      <c r="D149" t="n">
+        <v>-3.855596214896483</v>
+      </c>
+      <c r="E149" t="n">
+        <v>26.7588481016521</v>
+      </c>
+      <c r="F149" t="n">
+        <v>21.38480756210971</v>
+      </c>
+      <c r="G149" t="n">
+        <v>29.30881731975372</v>
+      </c>
+      <c r="H149" t="n">
+        <v>-92.46484551972567</v>
+      </c>
+      <c r="I149" t="n">
+        <v>6.700155728230888</v>
+      </c>
+      <c r="J149" t="n">
+        <v>26.69624430450378</v>
+      </c>
+      <c r="K149" t="n">
+        <v>9.250124946332502</v>
+      </c>
+      <c r="L149" t="n">
+        <v>-87.15340877733161</v>
+      </c>
+      <c r="M149" t="n">
+        <v>51.95155884910947</v>
+      </c>
+      <c r="N149" t="n">
+        <v>-143.2329800489664</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>9</v>
+      </c>
+      <c r="B150" t="n">
+        <v>6.092576980974942</v>
+      </c>
+      <c r="C150" t="n">
+        <v>28.57341936468722</v>
+      </c>
+      <c r="D150" t="n">
+        <v>-0.8471983293170848</v>
+      </c>
+      <c r="E150" t="n">
+        <v>27.38829075065058</v>
+      </c>
+      <c r="F150" t="n">
+        <v>24.37497386437376</v>
+      </c>
+      <c r="G150" t="n">
+        <v>31.72985101989372</v>
+      </c>
+      <c r="H150" t="n">
+        <v>-92.39805655114469</v>
+      </c>
+      <c r="I150" t="n">
+        <v>6.890575353137988</v>
+      </c>
+      <c r="J150" t="n">
+        <v>27.60083242955845</v>
+      </c>
+      <c r="K150" t="n">
+        <v>11.23213562238114</v>
+      </c>
+      <c r="L150" t="n">
+        <v>-89.17219798596</v>
+      </c>
+      <c r="M150" t="n">
+        <v>59.46079705231288</v>
+      </c>
+      <c r="N150" t="n">
+        <v>-140.5757677845704</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>10</v>
+      </c>
+      <c r="B151" t="n">
+        <v>6.42327094451071</v>
+      </c>
+      <c r="C151" t="n">
+        <v>28.65448941419694</v>
+      </c>
+      <c r="D151" t="n">
+        <v>2.361372157479072</v>
+      </c>
+      <c r="E151" t="n">
+        <v>27.71675508625803</v>
+      </c>
+      <c r="F151" t="n">
+        <v>27.59395336373311</v>
+      </c>
+      <c r="G151" t="n">
+        <v>31.15201945593522</v>
+      </c>
+      <c r="H151" t="n">
+        <v>-92.43618857736628</v>
+      </c>
+      <c r="I151" t="n">
+        <v>6.989942715170496</v>
+      </c>
+      <c r="J151" t="n">
+        <v>28.57464135373439</v>
+      </c>
+      <c r="K151" t="n">
+        <v>10.42520708484769</v>
+      </c>
+      <c r="L151" t="n">
+        <v>-91.45550058736501</v>
+      </c>
+      <c r="M151" t="n">
+        <v>63.95113646381277</v>
+      </c>
+      <c r="N151" t="n">
+        <v>-137.3173110126157</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>11</v>
+      </c>
+      <c r="B152" t="n">
+        <v>6.753964908046478</v>
+      </c>
+      <c r="C152" t="n">
+        <v>27.68934573084024</v>
+      </c>
+      <c r="D152" t="n">
+        <v>5.42241684714688</v>
+      </c>
+      <c r="E152" t="n">
+        <v>27.70295497348244</v>
+      </c>
+      <c r="F152" t="n">
+        <v>30.67241317959246</v>
+      </c>
+      <c r="G152" t="n">
+        <v>27.6530993321199</v>
+      </c>
+      <c r="H152" t="n">
+        <v>-92.49998656440459</v>
+      </c>
+      <c r="I152" t="n">
+        <v>6.985767891137545</v>
+      </c>
+      <c r="J152" t="n">
+        <v>29.50594012155738</v>
+      </c>
+      <c r="K152" t="n">
+        <v>6.935912249775004</v>
+      </c>
+      <c r="L152" t="n">
+        <v>-93.66645962243966</v>
+      </c>
+      <c r="M152" t="n">
+        <v>64.91463148210208</v>
+      </c>
+      <c r="N152" t="n">
+        <v>-133.7513556250811</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>12</v>
+      </c>
+      <c r="B153" t="n">
+        <v>7.084658871582246</v>
+      </c>
+      <c r="C153" t="n">
+        <v>25.78257660845605</v>
+      </c>
+      <c r="D153" t="n">
+        <v>8.004224050558687</v>
+      </c>
+      <c r="E153" t="n">
+        <v>27.45218503889162</v>
+      </c>
+      <c r="F153" t="n">
+        <v>33.19896373345715</v>
+      </c>
+      <c r="G153" t="n">
+        <v>21.33579771947419</v>
+      </c>
+      <c r="H153" t="n">
+        <v>-92.29756121457852</v>
+      </c>
+      <c r="I153" t="n">
+        <v>6.909904717647885</v>
+      </c>
+      <c r="J153" t="n">
+        <v>30.2702747428946</v>
+      </c>
+      <c r="K153" t="n">
+        <v>0.7935173982304526</v>
+      </c>
+      <c r="L153" t="n">
+        <v>-95.22625020514107</v>
+      </c>
+      <c r="M153" t="n">
+        <v>61.97895669814836</v>
+      </c>
+      <c r="N153" t="n">
+        <v>-130.22157545066</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>13</v>
+      </c>
+      <c r="B154" t="n">
+        <v>7.415352835118012</v>
+      </c>
+      <c r="C154" t="n">
+        <v>23.14081006802608</v>
+      </c>
+      <c r="D154" t="n">
+        <v>9.827014896358444</v>
+      </c>
+      <c r="E154" t="n">
+        <v>27.18896083043538</v>
+      </c>
+      <c r="F154" t="n">
+        <v>34.75039699840882</v>
+      </c>
+      <c r="G154" t="n">
+        <v>12.35910160180724</v>
+      </c>
+      <c r="H154" t="n">
+        <v>-91.3034789877093</v>
+      </c>
+      <c r="I154" t="n">
+        <v>6.830273864669527</v>
+      </c>
+      <c r="J154" t="n">
+        <v>30.7396158986783</v>
+      </c>
+      <c r="K154" t="n">
+        <v>-7.999585363958612</v>
+      </c>
+      <c r="L154" t="n">
+        <v>-95.31426008743982</v>
+      </c>
+      <c r="M154" t="n">
+        <v>54.95066653435794</v>
+      </c>
+      <c r="N154" t="n">
+        <v>-127.0254025661032</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>14</v>
+      </c>
+      <c r="B155" t="n">
+        <v>7.746046798653781</v>
+      </c>
+      <c r="C155" t="n">
+        <v>20.05032250543721</v>
+      </c>
+      <c r="D155" t="n">
+        <v>10.69326171288964</v>
+      </c>
+      <c r="E155" t="n">
+        <v>27.15436389024016</v>
+      </c>
+      <c r="F155" t="n">
+        <v>34.92330702863362</v>
+      </c>
+      <c r="G155" t="n">
+        <v>1.129657827100637</v>
+      </c>
+      <c r="H155" t="n">
+        <v>-88.7635323448047</v>
+      </c>
+      <c r="I155" t="n">
+        <v>6.819807563433999</v>
+      </c>
+      <c r="J155" t="n">
+        <v>30.79192481538496</v>
+      </c>
+      <c r="K155" t="n">
+        <v>-19.20489849970553</v>
+      </c>
+      <c r="L155" t="n">
+        <v>-92.89491455805336</v>
+      </c>
+      <c r="M155" t="n">
+        <v>43.93220829822495</v>
+      </c>
+      <c r="N155" t="n">
+        <v>-124.2323764295948</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>15</v>
+      </c>
+      <c r="B156" t="n">
+        <v>8.076740762189548</v>
+      </c>
+      <c r="C156" t="n">
+        <v>16.84601620195139</v>
+      </c>
+      <c r="D156" t="n">
+        <v>10.50909321637684</v>
+      </c>
+      <c r="E156" t="n">
+        <v>27.41683350686776</v>
+      </c>
+      <c r="F156" t="n">
+        <v>33.43986558684183</v>
+      </c>
+      <c r="G156" t="n">
+        <v>-11.30794275866747</v>
+      </c>
+      <c r="H156" t="n">
+        <v>-84.00381957497078</v>
+      </c>
+      <c r="I156" t="n">
+        <v>6.899210136531421</v>
+      </c>
+      <c r="J156" t="n">
+        <v>30.34315261450677</v>
+      </c>
+      <c r="K156" t="n">
+        <v>-31.8255661290038</v>
+      </c>
+      <c r="L156" t="n">
+        <v>-87.10053254730583</v>
+      </c>
+      <c r="M156" t="n">
+        <v>29.64423263539317</v>
+      </c>
+      <c r="N156" t="n">
+        <v>-121.5939320786384</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>16</v>
+      </c>
+      <c r="B157" t="n">
+        <v>8.407434725725317</v>
+      </c>
+      <c r="C157" t="n">
+        <v>13.87512746548638</v>
+      </c>
+      <c r="D157" t="n">
+        <v>9.294466921085883</v>
+      </c>
+      <c r="E157" t="n">
+        <v>27.71643859312513</v>
+      </c>
+      <c r="F157" t="n">
+        <v>30.41271983812198</v>
+      </c>
+      <c r="G157" t="n">
+        <v>-22.9893546467396</v>
+      </c>
+      <c r="H157" t="n">
+        <v>-77.36389682478573</v>
+      </c>
+      <c r="I157" t="n">
+        <v>6.989846969348777</v>
+      </c>
+      <c r="J157" t="n">
+        <v>29.42737743002009</v>
+      </c>
+      <c r="K157" t="n">
+        <v>-43.71594627051596</v>
+      </c>
+      <c r="L157" t="n">
+        <v>-78.34923923288761</v>
+      </c>
+      <c r="M157" t="n">
+        <v>13.91018148157017</v>
+      </c>
+      <c r="N157" t="n">
+        <v>-118.9393879350523</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>17</v>
+      </c>
+      <c r="B158" t="n">
+        <v>8.738128689261083</v>
+      </c>
+      <c r="C158" t="n">
+        <v>11.4595981887266</v>
+      </c>
+      <c r="D158" t="n">
+        <v>7.181006432980378</v>
+      </c>
+      <c r="E158" t="n">
+        <v>27.64956278225451</v>
+      </c>
+      <c r="F158" t="n">
+        <v>26.55747531821106</v>
+      </c>
+      <c r="G158" t="n">
+        <v>-31.66020850096656</v>
+      </c>
+      <c r="H158" t="n">
+        <v>-70.98310383698367</v>
+      </c>
+      <c r="I158" t="n">
+        <v>6.969615631606407</v>
+      </c>
+      <c r="J158" t="n">
+        <v>28.26108497021511</v>
+      </c>
+      <c r="K158" t="n">
+        <v>-52.34015565161467</v>
+      </c>
+      <c r="L158" t="n">
+        <v>-69.27949418497963</v>
+      </c>
+      <c r="M158" t="n">
+        <v>-0.4477646451716297</v>
+      </c>
+      <c r="N158" t="n">
+        <v>-116.9818057327236</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>18</v>
+      </c>
+      <c r="B159" t="n">
+        <v>9.068822652796852</v>
+      </c>
+      <c r="C159" t="n">
+        <v>9.861188449607457</v>
+      </c>
+      <c r="D159" t="n">
+        <v>4.397737989664864</v>
+      </c>
+      <c r="E159" t="n">
+        <v>27.10568952294837</v>
+      </c>
+      <c r="F159" t="n">
+        <v>22.84196968229831</v>
+      </c>
+      <c r="G159" t="n">
+        <v>-36.06723520117182</v>
+      </c>
+      <c r="H159" t="n">
+        <v>-67.56797748786511</v>
+      </c>
+      <c r="I159" t="n">
+        <v>6.805082544757491</v>
+      </c>
+      <c r="J159" t="n">
+        <v>27.13706645851041</v>
+      </c>
+      <c r="K159" t="n">
+        <v>-56.3678421793627</v>
+      </c>
+      <c r="L159" t="n">
+        <v>-63.272880711653</v>
+      </c>
+      <c r="M159" t="n">
+        <v>-10.8978968733922</v>
+      </c>
+      <c r="N159" t="n">
+        <v>-117.1320938997014</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>19</v>
+      </c>
+      <c r="B160" t="n">
+        <v>9.399516616332619</v>
+      </c>
+      <c r="C160" t="n">
+        <v>9.253110745245055</v>
+      </c>
+      <c r="D160" t="n">
+        <v>1.2462719138322</v>
+      </c>
+      <c r="E160" t="n">
+        <v>26.31194193651951</v>
+      </c>
+      <c r="F160" t="n">
+        <v>19.86236114835194</v>
+      </c>
+      <c r="G160" t="n">
+        <v>-36.18080599191165</v>
+      </c>
+      <c r="H160" t="n">
+        <v>-68.19755462150795</v>
+      </c>
+      <c r="I160" t="n">
+        <v>6.564957224493295</v>
+      </c>
+      <c r="J160" t="n">
+        <v>26.2356722801737</v>
+      </c>
+      <c r="K160" t="n">
+        <v>-55.92779070393787</v>
+      </c>
+      <c r="L160" t="n">
+        <v>-61.82424348968619</v>
+      </c>
+      <c r="M160" t="n">
+        <v>-16.27696982803617</v>
+      </c>
+      <c r="N160" t="n">
+        <v>-120.1006810543722</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>20</v>
+      </c>
+      <c r="B161" t="n">
+        <v>9.730210579868388</v>
+      </c>
+      <c r="C161" t="n">
+        <v>9.701259730204789</v>
+      </c>
+      <c r="D161" t="n">
+        <v>-1.931881545166664</v>
+      </c>
+      <c r="E161" t="n">
+        <v>25.53534878581116</v>
+      </c>
+      <c r="F161" t="n">
+        <v>17.73647181191756</v>
+      </c>
+      <c r="G161" t="n">
+        <v>-32.47072003175674</v>
+      </c>
+      <c r="H161" t="n">
+        <v>-72.05238358535806</v>
+      </c>
+      <c r="I161" t="n">
+        <v>6.330021481421864</v>
+      </c>
+      <c r="J161" t="n">
+        <v>25.59254609436162</v>
+      </c>
+      <c r="K161" t="n">
+        <v>-51.67604733614604</v>
+      </c>
+      <c r="L161" t="n">
+        <v>-64.196309302914</v>
+      </c>
+      <c r="M161" t="n">
+        <v>-16.57026598178295</v>
+      </c>
+      <c r="N161" t="n">
+        <v>-125.3184402119656</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>